<commit_message>
I added exception handling to handle the hangs when the vpn isn't working well. Added a time out to the stream reader to further prevent hanging
</commit_message>
<xml_diff>
--- a/StockPredictor/bin/Debug/Packages/Data/BIIB/BIIBBag.xlsx
+++ b/StockPredictor/bin/Debug/Packages/Data/BIIB/BIIBBag.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
   <si>
     <t>Date</t>
   </si>
@@ -384,13 +384,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
@@ -487,6 +487,88 @@
         <v>0</v>
       </c>
     </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>42600.834976851853</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3">
+        <v>7470</v>
+      </c>
+      <c r="D3">
+        <v>9083</v>
+      </c>
+      <c r="E3">
+        <v>1110</v>
+      </c>
+      <c r="F3">
+        <v>147</v>
+      </c>
+      <c r="G3">
+        <v>53</v>
+      </c>
+      <c r="H3">
+        <v>73</v>
+      </c>
+      <c r="I3">
+        <v>26</v>
+      </c>
+      <c r="J3">
+        <v>3</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>99</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>42600.879965277774</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4">
+        <v>6830</v>
+      </c>
+      <c r="D4">
+        <v>9265</v>
+      </c>
+      <c r="E4">
+        <v>1125</v>
+      </c>
+      <c r="F4">
+        <v>152</v>
+      </c>
+      <c r="G4">
+        <v>59</v>
+      </c>
+      <c r="H4">
+        <v>71</v>
+      </c>
+      <c r="I4">
+        <v>27</v>
+      </c>
+      <c r="J4">
+        <v>3</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>99</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
the user can now choose not to save the results of the search. The yahoo method that retrieves the compnay name threw an unhadled exception, that is now handled by the code
</commit_message>
<xml_diff>
--- a/StockPredictor/bin/Debug/Packages/Data/BIIB/BIIBBag.xlsx
+++ b/StockPredictor/bin/Debug/Packages/Data/BIIB/BIIBBag.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
   <si>
     <t>Date</t>
   </si>
@@ -384,7 +384,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M4"/>
+  <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -569,6 +569,47 @@
         <v>0</v>
       </c>
     </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>42602.583020833335</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5">
+        <v>6613</v>
+      </c>
+      <c r="D5">
+        <v>10320</v>
+      </c>
+      <c r="E5">
+        <v>1283</v>
+      </c>
+      <c r="F5">
+        <v>147</v>
+      </c>
+      <c r="G5">
+        <v>71</v>
+      </c>
+      <c r="H5">
+        <v>66</v>
+      </c>
+      <c r="I5">
+        <v>31</v>
+      </c>
+      <c r="J5">
+        <v>4</v>
+      </c>
+      <c r="K5">
+        <v>2</v>
+      </c>
+      <c r="L5">
+        <v>66</v>
+      </c>
+      <c r="M5">
+        <v>33</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
continued to train the program
</commit_message>
<xml_diff>
--- a/StockPredictor/bin/Debug/Packages/Data/BIIB/BIIBBag.xlsx
+++ b/StockPredictor/bin/Debug/Packages/Data/BIIB/BIIBBag.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
   <si>
     <t>Date</t>
   </si>
@@ -384,7 +384,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M5"/>
+  <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -610,6 +610,47 @@
         <v>33</v>
       </c>
     </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>42604.890810185185</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6">
+        <v>5007</v>
+      </c>
+      <c r="D6">
+        <v>6181</v>
+      </c>
+      <c r="E6">
+        <v>824</v>
+      </c>
+      <c r="F6">
+        <v>91</v>
+      </c>
+      <c r="G6">
+        <v>51</v>
+      </c>
+      <c r="H6">
+        <v>63</v>
+      </c>
+      <c r="I6">
+        <v>35</v>
+      </c>
+      <c r="J6">
+        <v>2</v>
+      </c>
+      <c r="K6">
+        <v>9</v>
+      </c>
+      <c r="L6">
+        <v>18</v>
+      </c>
+      <c r="M6">
+        <v>81</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
trader reads excel files for score. Overall this method is slow. It prevents trades if there is no sentiment information
</commit_message>
<xml_diff>
--- a/StockPredictor/bin/Debug/Packages/Data/BIIB/BIIBBag.xlsx
+++ b/StockPredictor/bin/Debug/Packages/Data/BIIB/BIIBBag.xlsx
@@ -24,45 +24,48 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Date</t>
   </si>
   <si>
+    <t>totalScore</t>
+  </si>
+  <si>
+    <t>posWordPercentage</t>
+  </si>
+  <si>
+    <t>negWordPercentage</t>
+  </si>
+  <si>
+    <t>posPhrasePercentage</t>
+  </si>
+  <si>
+    <t>negPhrasePercentage</t>
+  </si>
+  <si>
+    <t>ElapsedMs</t>
+  </si>
+  <si>
+    <t>wordCount</t>
+  </si>
+  <si>
+    <t>sentenceCount</t>
+  </si>
+  <si>
+    <t>posWordCount</t>
+  </si>
+  <si>
+    <t>negWordCount</t>
+  </si>
+  <si>
+    <t>positivePhraseCount</t>
+  </si>
+  <si>
+    <t>negativePhraseCount</t>
+  </si>
+  <si>
     <t>Method</t>
-  </si>
-  <si>
-    <t>ElapsedMs</t>
-  </si>
-  <si>
-    <t>wordCount</t>
-  </si>
-  <si>
-    <t>sentenceCount</t>
-  </si>
-  <si>
-    <t>posWordCount</t>
-  </si>
-  <si>
-    <t>negWordCount</t>
-  </si>
-  <si>
-    <t>posWordPercentage</t>
-  </si>
-  <si>
-    <t>negWordPercentage</t>
-  </si>
-  <si>
-    <t>positivePhraseCount</t>
-  </si>
-  <si>
-    <t>negativePhraseCount</t>
-  </si>
-  <si>
-    <t>posPhrasePercentage</t>
-  </si>
-  <si>
-    <t>negPhrasePercentage</t>
   </si>
   <si>
     <t>Bag</t>
@@ -384,28 +387,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M6"/>
+  <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -445,210 +448,52 @@
       <c r="M1" t="s">
         <v>12</v>
       </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>42587.798333333332</v>
-      </c>
-      <c r="B2" t="s">
-        <v>13</v>
+        <v>42605.53634259259</v>
+      </c>
+      <c r="B2">
+        <v>-30</v>
       </c>
       <c r="C2">
-        <v>1374</v>
+        <v>58</v>
       </c>
       <c r="D2">
-        <v>870</v>
+        <v>39</v>
       </c>
       <c r="E2">
-        <v>118</v>
+        <v>20</v>
       </c>
       <c r="F2">
-        <v>10</v>
+        <v>80</v>
       </c>
       <c r="G2">
-        <v>3</v>
+        <v>4170</v>
       </c>
       <c r="H2">
-        <v>76</v>
+        <v>6308</v>
       </c>
       <c r="I2">
-        <v>23</v>
+        <v>772</v>
       </c>
       <c r="J2">
-        <v>1</v>
+        <v>98</v>
       </c>
       <c r="K2">
-        <v>0</v>
+        <v>66</v>
       </c>
       <c r="L2">
-        <v>100</v>
+        <v>5</v>
       </c>
       <c r="M2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>42600.834976851853</v>
-      </c>
-      <c r="B3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3">
-        <v>7470</v>
-      </c>
-      <c r="D3">
-        <v>9083</v>
-      </c>
-      <c r="E3">
-        <v>1110</v>
-      </c>
-      <c r="F3">
-        <v>147</v>
-      </c>
-      <c r="G3">
-        <v>53</v>
-      </c>
-      <c r="H3">
-        <v>73</v>
-      </c>
-      <c r="I3">
-        <v>26</v>
-      </c>
-      <c r="J3">
-        <v>3</v>
-      </c>
-      <c r="K3">
-        <v>0</v>
-      </c>
-      <c r="L3">
-        <v>99</v>
-      </c>
-      <c r="M3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>42600.879965277774</v>
-      </c>
-      <c r="B4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4">
-        <v>6830</v>
-      </c>
-      <c r="D4">
-        <v>9265</v>
-      </c>
-      <c r="E4">
-        <v>1125</v>
-      </c>
-      <c r="F4">
-        <v>152</v>
-      </c>
-      <c r="G4">
-        <v>59</v>
-      </c>
-      <c r="H4">
-        <v>71</v>
-      </c>
-      <c r="I4">
-        <v>27</v>
-      </c>
-      <c r="J4">
-        <v>3</v>
-      </c>
-      <c r="K4">
-        <v>0</v>
-      </c>
-      <c r="L4">
-        <v>99</v>
-      </c>
-      <c r="M4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>42602.583020833335</v>
-      </c>
-      <c r="B5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5">
-        <v>6613</v>
-      </c>
-      <c r="D5">
-        <v>10320</v>
-      </c>
-      <c r="E5">
-        <v>1283</v>
-      </c>
-      <c r="F5">
-        <v>147</v>
-      </c>
-      <c r="G5">
-        <v>71</v>
-      </c>
-      <c r="H5">
-        <v>66</v>
-      </c>
-      <c r="I5">
-        <v>31</v>
-      </c>
-      <c r="J5">
-        <v>4</v>
-      </c>
-      <c r="K5">
-        <v>2</v>
-      </c>
-      <c r="L5">
-        <v>66</v>
-      </c>
-      <c r="M5">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>42604.890810185185</v>
-      </c>
-      <c r="B6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6">
-        <v>5007</v>
-      </c>
-      <c r="D6">
-        <v>6181</v>
-      </c>
-      <c r="E6">
-        <v>824</v>
-      </c>
-      <c r="F6">
-        <v>91</v>
-      </c>
-      <c r="G6">
-        <v>51</v>
-      </c>
-      <c r="H6">
-        <v>63</v>
-      </c>
-      <c r="I6">
-        <v>35</v>
-      </c>
-      <c r="J6">
-        <v>2</v>
-      </c>
-      <c r="K6">
-        <v>9</v>
-      </c>
-      <c r="L6">
-        <v>18</v>
-      </c>
-      <c r="M6">
-        <v>81</v>
+        <v>20</v>
+      </c>
+      <c r="N2" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed some issues with the trading. added a retry feature to the sentiment analysis
</commit_message>
<xml_diff>
--- a/StockPredictor/bin/Debug/Packages/Data/BIIB/BIIBBag.xlsx
+++ b/StockPredictor/bin/Debug/Packages/Data/BIIB/BIIBBag.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t>Date</t>
   </si>
@@ -387,7 +387,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N2"/>
+  <dimension ref="A1:N3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -496,6 +496,50 @@
         <v>14</v>
       </c>
     </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>42605.648333333331</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>24</v>
+      </c>
+      <c r="H3">
+        <v>4</v>
+      </c>
+      <c r="I3">
+        <v>2</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="N3" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
changed the trading and excel classes. Updated trader so as one can retry. It also checks the date is correct and allows for manual input. The trader class will now pass an excel application object. This speeds up the application as the the excel classes isn't constantly opening and closing excel application objects
</commit_message>
<xml_diff>
--- a/StockPredictor/bin/Debug/Packages/Data/BIIB/BIIBBag.xlsx
+++ b/StockPredictor/bin/Debug/Packages/Data/BIIB/BIIBBag.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
   <si>
     <t>Date</t>
   </si>
@@ -387,7 +387,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N3"/>
+  <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -540,6 +540,50 @@
         <v>14</v>
       </c>
     </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>42605.886620370373</v>
+      </c>
+      <c r="B4">
+        <v>-28</v>
+      </c>
+      <c r="C4">
+        <v>49</v>
+      </c>
+      <c r="D4">
+        <v>48</v>
+      </c>
+      <c r="E4">
+        <v>22</v>
+      </c>
+      <c r="F4">
+        <v>77</v>
+      </c>
+      <c r="G4">
+        <v>15700</v>
+      </c>
+      <c r="H4">
+        <v>8713</v>
+      </c>
+      <c r="I4">
+        <v>1089</v>
+      </c>
+      <c r="J4">
+        <v>105</v>
+      </c>
+      <c r="K4">
+        <v>104</v>
+      </c>
+      <c r="L4">
+        <v>6</v>
+      </c>
+      <c r="M4">
+        <v>21</v>
+      </c>
+      <c r="N4" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
fixed bugs with the manual trading. A few lines of code where needed
</commit_message>
<xml_diff>
--- a/StockPredictor/bin/Debug/Packages/Data/BIIB/BIIBBag.xlsx
+++ b/StockPredictor/bin/Debug/Packages/Data/BIIB/BIIBBag.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
   <si>
     <t>Date</t>
   </si>
@@ -387,7 +387,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N4"/>
+  <dimension ref="A1:N5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -584,6 +584,50 @@
         <v>14</v>
       </c>
     </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>42606.88175925926</v>
+      </c>
+      <c r="B5">
+        <v>32</v>
+      </c>
+      <c r="C5">
+        <v>68</v>
+      </c>
+      <c r="D5">
+        <v>29</v>
+      </c>
+      <c r="E5">
+        <v>58</v>
+      </c>
+      <c r="F5">
+        <v>41</v>
+      </c>
+      <c r="G5">
+        <v>7959</v>
+      </c>
+      <c r="H5">
+        <v>13770</v>
+      </c>
+      <c r="I5">
+        <v>1678</v>
+      </c>
+      <c r="J5">
+        <v>222</v>
+      </c>
+      <c r="K5">
+        <v>95</v>
+      </c>
+      <c r="L5">
+        <v>7</v>
+      </c>
+      <c r="M5">
+        <v>5</v>
+      </c>
+      <c r="N5" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
fixed a bug with the 20 minute trade. Now you don't need to enter the close price if the trader can't locate data from yahoo
</commit_message>
<xml_diff>
--- a/StockPredictor/bin/Debug/Packages/Data/BIIB/BIIBBag.xlsx
+++ b/StockPredictor/bin/Debug/Packages/Data/BIIB/BIIBBag.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
   <si>
     <t>Date</t>
   </si>
@@ -387,7 +387,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N5"/>
+  <dimension ref="A1:N6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -628,6 +628,50 @@
         <v>14</v>
       </c>
     </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>42607.889189814814</v>
+      </c>
+      <c r="B6">
+        <v>-8</v>
+      </c>
+      <c r="C6">
+        <v>57</v>
+      </c>
+      <c r="D6">
+        <v>39</v>
+      </c>
+      <c r="E6">
+        <v>31</v>
+      </c>
+      <c r="F6">
+        <v>68</v>
+      </c>
+      <c r="G6">
+        <v>38807</v>
+      </c>
+      <c r="H6">
+        <v>31379</v>
+      </c>
+      <c r="I6">
+        <v>3781</v>
+      </c>
+      <c r="J6">
+        <v>380</v>
+      </c>
+      <c r="K6">
+        <v>261</v>
+      </c>
+      <c r="L6">
+        <v>14</v>
+      </c>
+      <c r="M6">
+        <v>31</v>
+      </c>
+      <c r="N6" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Disabled hosting in debug-> settings because debug wasn't working on the background thread
</commit_message>
<xml_diff>
--- a/StockPredictor/bin/Debug/Packages/Data/BIIB/BIIBBag.xlsx
+++ b/StockPredictor/bin/Debug/Packages/Data/BIIB/BIIBBag.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
   <si>
     <t>Date</t>
   </si>
@@ -387,7 +387,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N6"/>
+  <dimension ref="A1:N7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -672,6 +672,50 @@
         <v>14</v>
       </c>
     </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>42608.892002314817</v>
+      </c>
+      <c r="B7">
+        <v>4</v>
+      </c>
+      <c r="C7">
+        <v>56</v>
+      </c>
+      <c r="D7">
+        <v>41</v>
+      </c>
+      <c r="E7">
+        <v>47</v>
+      </c>
+      <c r="F7">
+        <v>52</v>
+      </c>
+      <c r="G7">
+        <v>16433</v>
+      </c>
+      <c r="H7">
+        <v>30718</v>
+      </c>
+      <c r="I7">
+        <v>3524</v>
+      </c>
+      <c r="J7">
+        <v>378</v>
+      </c>
+      <c r="K7">
+        <v>278</v>
+      </c>
+      <c r="L7">
+        <v>17</v>
+      </c>
+      <c r="M7">
+        <v>19</v>
+      </c>
+      <c r="N7" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added a message that tels the user what time the program will execute after a delay
</commit_message>
<xml_diff>
--- a/StockPredictor/bin/Debug/Packages/Data/BIIB/BIIBBag.xlsx
+++ b/StockPredictor/bin/Debug/Packages/Data/BIIB/BIIBBag.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="15">
   <si>
     <t>Date</t>
   </si>
@@ -387,7 +387,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N7"/>
+  <dimension ref="A1:N8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -716,6 +716,50 @@
         <v>14</v>
       </c>
     </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>42611.885659722226</v>
+      </c>
+      <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="C8">
+        <v>52</v>
+      </c>
+      <c r="D8">
+        <v>43</v>
+      </c>
+      <c r="E8">
+        <v>47</v>
+      </c>
+      <c r="F8">
+        <v>52</v>
+      </c>
+      <c r="G8">
+        <v>10427</v>
+      </c>
+      <c r="H8">
+        <v>19550</v>
+      </c>
+      <c r="I8">
+        <v>2478</v>
+      </c>
+      <c r="J8">
+        <v>239</v>
+      </c>
+      <c r="K8">
+        <v>198</v>
+      </c>
+      <c r="L8">
+        <v>11</v>
+      </c>
+      <c r="M8">
+        <v>12</v>
+      </c>
+      <c r="N8" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
made the excel single threaded. This may help with the random exceptions the program has been experiencing
</commit_message>
<xml_diff>
--- a/StockPredictor/bin/Debug/Packages/Data/BIIB/BIIBBag.xlsx
+++ b/StockPredictor/bin/Debug/Packages/Data/BIIB/BIIBBag.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="15">
   <si>
     <t>Date</t>
   </si>
@@ -387,7 +387,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N8"/>
+  <dimension ref="A1:N9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -760,6 +760,50 @@
         <v>14</v>
       </c>
     </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>42612.892488425925</v>
+      </c>
+      <c r="B9">
+        <v>20</v>
+      </c>
+      <c r="C9">
+        <v>54</v>
+      </c>
+      <c r="D9">
+        <v>41</v>
+      </c>
+      <c r="E9">
+        <v>82</v>
+      </c>
+      <c r="F9">
+        <v>17</v>
+      </c>
+      <c r="G9">
+        <v>13103</v>
+      </c>
+      <c r="H9">
+        <v>26404</v>
+      </c>
+      <c r="I9">
+        <v>3223</v>
+      </c>
+      <c r="J9">
+        <v>364</v>
+      </c>
+      <c r="K9">
+        <v>279</v>
+      </c>
+      <c r="L9">
+        <v>24</v>
+      </c>
+      <c r="M9">
+        <v>5</v>
+      </c>
+      <c r="N9" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
updated data, updated word lists
</commit_message>
<xml_diff>
--- a/StockPredictor/bin/Debug/Packages/Data/BIIB/BIIBBag.xlsx
+++ b/StockPredictor/bin/Debug/Packages/Data/BIIB/BIIBBag.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="15">
   <si>
     <t>Date</t>
   </si>
@@ -387,7 +387,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N9"/>
+  <dimension ref="A1:N13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -804,6 +804,182 @@
         <v>14</v>
       </c>
     </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>42613.759386574071</v>
+      </c>
+      <c r="B10">
+        <v>14</v>
+      </c>
+      <c r="C10">
+        <v>54</v>
+      </c>
+      <c r="D10">
+        <v>43</v>
+      </c>
+      <c r="E10">
+        <v>54</v>
+      </c>
+      <c r="F10">
+        <v>23</v>
+      </c>
+      <c r="G10">
+        <v>16350</v>
+      </c>
+      <c r="H10">
+        <v>24762</v>
+      </c>
+      <c r="I10">
+        <v>2820</v>
+      </c>
+      <c r="J10">
+        <v>363</v>
+      </c>
+      <c r="K10">
+        <v>291</v>
+      </c>
+      <c r="L10">
+        <v>35</v>
+      </c>
+      <c r="M10">
+        <v>11</v>
+      </c>
+      <c r="N10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>42613.888055555559</v>
+      </c>
+      <c r="B11">
+        <v>20</v>
+      </c>
+      <c r="C11">
+        <v>55</v>
+      </c>
+      <c r="D11">
+        <v>40</v>
+      </c>
+      <c r="E11">
+        <v>55</v>
+      </c>
+      <c r="F11">
+        <v>24</v>
+      </c>
+      <c r="G11">
+        <v>17631</v>
+      </c>
+      <c r="H11">
+        <v>24259</v>
+      </c>
+      <c r="I11">
+        <v>2694</v>
+      </c>
+      <c r="J11">
+        <v>345</v>
+      </c>
+      <c r="K11">
+        <v>251</v>
+      </c>
+      <c r="L11">
+        <v>44</v>
+      </c>
+      <c r="M11">
+        <v>14</v>
+      </c>
+      <c r="N11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>42614.886192129627</v>
+      </c>
+      <c r="B12">
+        <v>24</v>
+      </c>
+      <c r="C12">
+        <v>53</v>
+      </c>
+      <c r="D12">
+        <v>40</v>
+      </c>
+      <c r="E12">
+        <v>53</v>
+      </c>
+      <c r="F12">
+        <v>16</v>
+      </c>
+      <c r="G12">
+        <v>33815</v>
+      </c>
+      <c r="H12">
+        <v>24993</v>
+      </c>
+      <c r="I12">
+        <v>2849</v>
+      </c>
+      <c r="J12">
+        <v>337</v>
+      </c>
+      <c r="K12">
+        <v>256</v>
+      </c>
+      <c r="L12">
+        <v>31</v>
+      </c>
+      <c r="M12">
+        <v>6</v>
+      </c>
+      <c r="N12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>42615.885671296295</v>
+      </c>
+      <c r="B13">
+        <v>16</v>
+      </c>
+      <c r="C13">
+        <v>53</v>
+      </c>
+      <c r="D13">
+        <v>42</v>
+      </c>
+      <c r="E13">
+        <v>53</v>
+      </c>
+      <c r="F13">
+        <v>30</v>
+      </c>
+      <c r="G13">
+        <v>10559</v>
+      </c>
+      <c r="H13">
+        <v>21629</v>
+      </c>
+      <c r="I13">
+        <v>2314</v>
+      </c>
+      <c r="J13">
+        <v>295</v>
+      </c>
+      <c r="K13">
+        <v>238</v>
+      </c>
+      <c r="L13">
+        <v>20</v>
+      </c>
+      <c r="M13">
+        <v>9</v>
+      </c>
+      <c r="N13" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
I changed the postagger classes. Now they share instances of the classes used to improve efficencies
</commit_message>
<xml_diff>
--- a/StockPredictor/bin/Debug/Packages/Data/BIIB/BIIBBag.xlsx
+++ b/StockPredictor/bin/Debug/Packages/Data/BIIB/BIIBBag.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="15">
   <si>
     <t>Date</t>
   </si>
@@ -387,7 +387,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N13"/>
+  <dimension ref="A1:N14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -980,6 +980,50 @@
         <v>14</v>
       </c>
     </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>42619.89266203704</v>
+      </c>
+      <c r="B14">
+        <v>26</v>
+      </c>
+      <c r="C14">
+        <v>63</v>
+      </c>
+      <c r="D14">
+        <v>34</v>
+      </c>
+      <c r="E14">
+        <v>63</v>
+      </c>
+      <c r="F14">
+        <v>32</v>
+      </c>
+      <c r="G14">
+        <v>13111</v>
+      </c>
+      <c r="H14">
+        <v>25133</v>
+      </c>
+      <c r="I14">
+        <v>2818</v>
+      </c>
+      <c r="J14">
+        <v>426</v>
+      </c>
+      <c r="K14">
+        <v>230</v>
+      </c>
+      <c r="L14">
+        <v>34</v>
+      </c>
+      <c r="M14">
+        <v>16</v>
+      </c>
+      <c r="N14" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
removed the ugly red scan button and replaced it with a blue one
</commit_message>
<xml_diff>
--- a/StockPredictor/bin/Debug/Packages/Data/BIIB/BIIBBag.xlsx
+++ b/StockPredictor/bin/Debug/Packages/Data/BIIB/BIIBBag.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="15">
   <si>
     <t>Date</t>
   </si>
@@ -387,7 +387,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N14"/>
+  <dimension ref="A1:N15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1024,6 +1024,50 @@
         <v>14</v>
       </c>
     </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>42620.888136574074</v>
+      </c>
+      <c r="B15">
+        <v>16</v>
+      </c>
+      <c r="C15">
+        <v>62</v>
+      </c>
+      <c r="D15">
+        <v>36</v>
+      </c>
+      <c r="E15">
+        <v>62</v>
+      </c>
+      <c r="F15">
+        <v>23</v>
+      </c>
+      <c r="G15">
+        <v>34074</v>
+      </c>
+      <c r="H15">
+        <v>27720</v>
+      </c>
+      <c r="I15">
+        <v>3249</v>
+      </c>
+      <c r="J15">
+        <v>393</v>
+      </c>
+      <c r="K15">
+        <v>225</v>
+      </c>
+      <c r="L15">
+        <v>30</v>
+      </c>
+      <c r="M15">
+        <v>9</v>
+      </c>
+      <c r="N15" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
fixed calculator bugs, rounded trend
</commit_message>
<xml_diff>
--- a/StockPredictor/bin/Debug/Packages/Data/BIIB/BIIBBag.xlsx
+++ b/StockPredictor/bin/Debug/Packages/Data/BIIB/BIIBBag.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="15">
   <si>
     <t>Date</t>
   </si>
@@ -387,7 +387,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N16"/>
+  <dimension ref="A1:N17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1112,6 +1112,50 @@
         <v>14</v>
       </c>
     </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>42622.888495370367</v>
+      </c>
+      <c r="B17">
+        <v>-10</v>
+      </c>
+      <c r="C17">
+        <v>58</v>
+      </c>
+      <c r="D17">
+        <v>39</v>
+      </c>
+      <c r="E17">
+        <v>58</v>
+      </c>
+      <c r="F17">
+        <v>27</v>
+      </c>
+      <c r="G17">
+        <v>10384</v>
+      </c>
+      <c r="H17">
+        <v>18782</v>
+      </c>
+      <c r="I17">
+        <v>2082</v>
+      </c>
+      <c r="J17">
+        <v>293</v>
+      </c>
+      <c r="K17">
+        <v>198</v>
+      </c>
+      <c r="L17">
+        <v>35</v>
+      </c>
+      <c r="M17">
+        <v>13</v>
+      </c>
+      <c r="N17" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
updated display text and changed calcualtor method for greater acuracy
</commit_message>
<xml_diff>
--- a/StockPredictor/bin/Debug/Packages/Data/BIIB/BIIBBag.xlsx
+++ b/StockPredictor/bin/Debug/Packages/Data/BIIB/BIIBBag.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="15">
   <si>
     <t>Date</t>
   </si>
@@ -387,7 +387,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N17"/>
+  <dimension ref="A1:N18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1156,6 +1156,50 @@
         <v>14</v>
       </c>
     </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>42625.885057870371</v>
+      </c>
+      <c r="B18">
+        <v>-26</v>
+      </c>
+      <c r="C18">
+        <v>63</v>
+      </c>
+      <c r="D18">
+        <v>35</v>
+      </c>
+      <c r="E18">
+        <v>80</v>
+      </c>
+      <c r="F18">
+        <v>20</v>
+      </c>
+      <c r="G18">
+        <v>6649</v>
+      </c>
+      <c r="H18">
+        <v>11170</v>
+      </c>
+      <c r="I18">
+        <v>1190</v>
+      </c>
+      <c r="J18">
+        <v>227</v>
+      </c>
+      <c r="K18">
+        <v>127</v>
+      </c>
+      <c r="L18">
+        <v>16</v>
+      </c>
+      <c r="M18">
+        <v>4</v>
+      </c>
+      <c r="N18" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
ticker appears with results
</commit_message>
<xml_diff>
--- a/StockPredictor/bin/Debug/Packages/Data/BIIB/BIIBBag.xlsx
+++ b/StockPredictor/bin/Debug/Packages/Data/BIIB/BIIBBag.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="27">
   <si>
     <t>Date</t>
   </si>
@@ -102,6 +102,9 @@
   </si>
   <si>
     <t>N/A</t>
+  </si>
+  <si>
+    <t>Neutral</t>
   </si>
 </sst>
 </file>
@@ -421,7 +424,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W2"/>
+  <dimension ref="A1:W3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -429,7 +432,7 @@
   <cols>
     <col min="1" max="1" width="14.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.5703125" bestFit="1" customWidth="1"/>
@@ -584,6 +587,77 @@
         <v>0</v>
       </c>
     </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>42632.882164351853</v>
+      </c>
+      <c r="B3">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3">
+        <v>14</v>
+      </c>
+      <c r="E3">
+        <v>12000</v>
+      </c>
+      <c r="F3">
+        <v>1284</v>
+      </c>
+      <c r="G3">
+        <v>58</v>
+      </c>
+      <c r="H3">
+        <v>39</v>
+      </c>
+      <c r="I3">
+        <v>70</v>
+      </c>
+      <c r="J3">
+        <v>29</v>
+      </c>
+      <c r="K3">
+        <v>7229</v>
+      </c>
+      <c r="L3">
+        <v>151</v>
+      </c>
+      <c r="M3">
+        <v>100</v>
+      </c>
+      <c r="N3">
+        <v>12</v>
+      </c>
+      <c r="O3">
+        <v>5</v>
+      </c>
+      <c r="P3" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q3">
+        <v>0</v>
+      </c>
+      <c r="R3">
+        <v>1.77</v>
+      </c>
+      <c r="S3" s="2">
+        <v>0.1132</v>
+      </c>
+      <c r="T3">
+        <v>-4.05</v>
+      </c>
+      <c r="U3">
+        <v>5.85</v>
+      </c>
+      <c r="V3" t="s">
+        <v>25</v>
+      </c>
+      <c r="W3">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
traded. Fixed 20 minute trade problem
</commit_message>
<xml_diff>
--- a/StockPredictor/bin/Debug/Packages/Data/BIIB/BIIBBag.xlsx
+++ b/StockPredictor/bin/Debug/Packages/Data/BIIB/BIIBBag.xlsx
@@ -439,19 +439,19 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.25" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.25" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
moved against was creating false psoitives
</commit_message>
<xml_diff>
--- a/StockPredictor/bin/Debug/Packages/Data/BIIB/BIIBBag.xlsx
+++ b/StockPredictor/bin/Debug/Packages/Data/BIIB/BIIBBag.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="31">
   <si>
     <t>Date</t>
   </si>
@@ -114,6 +114,9 @@
   </si>
   <si>
     <t>Down</t>
+  </si>
+  <si>
+    <t>Up</t>
   </si>
 </sst>
 </file>
@@ -433,25 +436,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y3"/>
+  <dimension ref="A1:Y4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.25" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.25" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.25">
@@ -678,6 +681,83 @@
       <c r="W3">
         <v>0</v>
       </c>
+      <c r="X3">
+        <v>4.75</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>42641.891493055555</v>
+      </c>
+      <c r="B4">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4">
+        <v>-4</v>
+      </c>
+      <c r="E4">
+        <v>14968</v>
+      </c>
+      <c r="F4">
+        <v>1683</v>
+      </c>
+      <c r="G4">
+        <v>60</v>
+      </c>
+      <c r="H4">
+        <v>37</v>
+      </c>
+      <c r="I4">
+        <v>42</v>
+      </c>
+      <c r="J4">
+        <v>57</v>
+      </c>
+      <c r="K4">
+        <v>8103</v>
+      </c>
+      <c r="L4">
+        <v>207</v>
+      </c>
+      <c r="M4">
+        <v>129</v>
+      </c>
+      <c r="N4">
+        <v>12</v>
+      </c>
+      <c r="O4">
+        <v>16</v>
+      </c>
+      <c r="P4" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q4">
+        <v>57.519894101767122</v>
+      </c>
+      <c r="R4">
+        <v>1.83</v>
+      </c>
+      <c r="S4" s="2">
+        <v>0.13639999999999999</v>
+      </c>
+      <c r="T4" s="2">
+        <v>1.6500000000000001E-2</v>
+      </c>
+      <c r="U4">
+        <v>6.04</v>
+      </c>
+      <c r="V4" t="s">
+        <v>27</v>
+      </c>
+      <c r="W4">
+        <v>2</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
removed false start data
</commit_message>
<xml_diff>
--- a/StockPredictor/bin/Debug/Packages/Data/BIIB/BIIBBag.xlsx
+++ b/StockPredictor/bin/Debug/Packages/Data/BIIB/BIIBBag.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VisualStudioProjects\StockPredictor\StockPredictor\bin\Debug\packages\Data\BIIB\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VisualStudioProjects\StockPredictor\StockPredictor\bin\Debug\Packages\Data\BIIB\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
   <si>
     <t>Date</t>
   </si>
@@ -110,13 +110,7 @@
     <t>N/A</t>
   </si>
   <si>
-    <t>Sell</t>
-  </si>
-  <si>
     <t>Down</t>
-  </si>
-  <si>
-    <t>Up</t>
   </si>
   <si>
     <t>Buy</t>
@@ -439,9 +433,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y5"/>
+  <dimension ref="A1:Y3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" activeCellId="1" sqref="A2:XFD2 A3:XFD3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -539,67 +535,67 @@
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>42639.882696759261</v>
+        <v>42641.891493055555</v>
       </c>
       <c r="B2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
         <v>25</v>
       </c>
       <c r="D2">
-        <v>-20</v>
+        <v>-4</v>
       </c>
       <c r="E2">
-        <v>17202</v>
+        <v>14968</v>
       </c>
       <c r="F2">
-        <v>1875</v>
+        <v>1683</v>
       </c>
       <c r="G2">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="H2">
+        <v>37</v>
+      </c>
+      <c r="I2">
         <v>42</v>
       </c>
-      <c r="I2">
-        <v>27</v>
-      </c>
       <c r="J2">
-        <v>72</v>
+        <v>57</v>
       </c>
       <c r="K2">
-        <v>11944</v>
+        <v>8103</v>
       </c>
       <c r="L2">
-        <v>233</v>
+        <v>207</v>
       </c>
       <c r="M2">
-        <v>186</v>
+        <v>129</v>
       </c>
       <c r="N2">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="O2">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="P2" t="s">
         <v>26</v>
       </c>
       <c r="Q2">
-        <v>57.931464516756321</v>
+        <v>57.519894101767122</v>
       </c>
       <c r="R2">
         <v>1.83</v>
       </c>
       <c r="S2" s="2">
-        <v>0.13370000000000001</v>
+        <v>0.13639999999999999</v>
       </c>
       <c r="T2" s="2">
-        <v>9.7999999999999997E-3</v>
+        <v>1.6500000000000001E-2</v>
       </c>
       <c r="U2">
-        <v>6.01</v>
+        <v>6.04</v>
       </c>
       <c r="V2" t="s">
         <v>27</v>
@@ -608,63 +604,63 @@
         <v>2</v>
       </c>
       <c r="X2">
-        <v>-1.8800050000000397</v>
+        <v>-5.4400019999999927</v>
       </c>
       <c r="Y2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>42640.883576388886</v>
+        <v>42642.883715277778</v>
       </c>
       <c r="B3">
-        <v>-8</v>
+        <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D3">
-        <v>-40</v>
+        <v>26</v>
       </c>
       <c r="E3">
-        <v>27569</v>
+        <v>24784</v>
       </c>
       <c r="F3">
-        <v>3012</v>
+        <v>2744</v>
       </c>
       <c r="G3">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="H3">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="I3">
-        <v>32</v>
+        <v>83</v>
       </c>
       <c r="J3">
-        <v>66</v>
+        <v>16</v>
       </c>
       <c r="K3">
-        <v>14004</v>
+        <v>19791</v>
       </c>
       <c r="L3">
-        <v>341</v>
+        <v>351</v>
       </c>
       <c r="M3">
-        <v>303</v>
+        <v>230</v>
       </c>
       <c r="N3">
-        <v>43</v>
+        <v>56</v>
       </c>
       <c r="O3">
-        <v>89</v>
+        <v>11</v>
       </c>
       <c r="P3" t="s">
         <v>26</v>
       </c>
       <c r="Q3">
-        <v>54.986430949289058</v>
+        <v>55.174763163562879</v>
       </c>
       <c r="R3">
         <v>1.8</v>
@@ -673,169 +669,15 @@
         <v>0.121</v>
       </c>
       <c r="T3" s="2">
-        <v>1.4E-3</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="U3">
-        <v>5.95</v>
+        <v>5.97</v>
       </c>
       <c r="V3" t="s">
         <v>27</v>
       </c>
       <c r="W3">
-        <v>0</v>
-      </c>
-      <c r="X3">
-        <v>4.75</v>
-      </c>
-      <c r="Y3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>42641.891493055555</v>
-      </c>
-      <c r="B4">
-        <v>4</v>
-      </c>
-      <c r="C4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D4">
-        <v>-4</v>
-      </c>
-      <c r="E4">
-        <v>14968</v>
-      </c>
-      <c r="F4">
-        <v>1683</v>
-      </c>
-      <c r="G4">
-        <v>60</v>
-      </c>
-      <c r="H4">
-        <v>37</v>
-      </c>
-      <c r="I4">
-        <v>42</v>
-      </c>
-      <c r="J4">
-        <v>57</v>
-      </c>
-      <c r="K4">
-        <v>8103</v>
-      </c>
-      <c r="L4">
-        <v>207</v>
-      </c>
-      <c r="M4">
-        <v>129</v>
-      </c>
-      <c r="N4">
-        <v>12</v>
-      </c>
-      <c r="O4">
-        <v>16</v>
-      </c>
-      <c r="P4" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q4">
-        <v>57.519894101767122</v>
-      </c>
-      <c r="R4">
-        <v>1.83</v>
-      </c>
-      <c r="S4" s="2">
-        <v>0.13639999999999999</v>
-      </c>
-      <c r="T4" s="2">
-        <v>1.6500000000000001E-2</v>
-      </c>
-      <c r="U4">
-        <v>6.04</v>
-      </c>
-      <c r="V4" t="s">
-        <v>27</v>
-      </c>
-      <c r="W4">
-        <v>2</v>
-      </c>
-      <c r="X4">
-        <v>-5.4400019999999927</v>
-      </c>
-      <c r="Y4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>42642.883715277778</v>
-      </c>
-      <c r="B5">
-        <v>8</v>
-      </c>
-      <c r="C5" t="s">
-        <v>31</v>
-      </c>
-      <c r="D5">
-        <v>26</v>
-      </c>
-      <c r="E5">
-        <v>24784</v>
-      </c>
-      <c r="F5">
-        <v>2744</v>
-      </c>
-      <c r="G5">
-        <v>59</v>
-      </c>
-      <c r="H5">
-        <v>39</v>
-      </c>
-      <c r="I5">
-        <v>83</v>
-      </c>
-      <c r="J5">
-        <v>16</v>
-      </c>
-      <c r="K5">
-        <v>19791</v>
-      </c>
-      <c r="L5">
-        <v>351</v>
-      </c>
-      <c r="M5">
-        <v>230</v>
-      </c>
-      <c r="N5">
-        <v>56</v>
-      </c>
-      <c r="O5">
-        <v>11</v>
-      </c>
-      <c r="P5" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q5">
-        <v>55.174763163562879</v>
-      </c>
-      <c r="R5">
-        <v>1.8</v>
-      </c>
-      <c r="S5" s="2">
-        <v>0.121</v>
-      </c>
-      <c r="T5" s="2">
-        <v>4.0000000000000001E-3</v>
-      </c>
-      <c r="U5">
-        <v>5.97</v>
-      </c>
-      <c r="V5" t="s">
-        <v>27</v>
-      </c>
-      <c r="W5">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
ran scans. Added words. Slight caluclation change
</commit_message>
<xml_diff>
--- a/StockPredictor/bin/Debug/Packages/Data/BIIB/BIIBBag.xlsx
+++ b/StockPredictor/bin/Debug/Packages/Data/BIIB/BIIBBag.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="32">
   <si>
     <t>Date</t>
   </si>
@@ -439,7 +439,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y5"/>
+  <dimension ref="A1:Y6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A3" activeCellId="1" sqref="A2:XFD2 A3:XFD3"/>
@@ -840,6 +840,83 @@
       <c r="W5">
         <v>2</v>
       </c>
+      <c r="X5">
+        <v>-1.4100040000000149</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>42647.885428240741</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6">
+        <v>6</v>
+      </c>
+      <c r="E6">
+        <v>18709</v>
+      </c>
+      <c r="F6">
+        <v>2107</v>
+      </c>
+      <c r="G6">
+        <v>55</v>
+      </c>
+      <c r="H6">
+        <v>43</v>
+      </c>
+      <c r="I6">
+        <v>67</v>
+      </c>
+      <c r="J6">
+        <v>31</v>
+      </c>
+      <c r="K6">
+        <v>23476</v>
+      </c>
+      <c r="L6">
+        <v>263</v>
+      </c>
+      <c r="M6">
+        <v>209</v>
+      </c>
+      <c r="N6">
+        <v>79</v>
+      </c>
+      <c r="O6">
+        <v>37</v>
+      </c>
+      <c r="P6" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q6">
+        <v>60.94594728999143</v>
+      </c>
+      <c r="R6">
+        <v>0</v>
+      </c>
+      <c r="S6" s="2">
+        <v>0.11890000000000001</v>
+      </c>
+      <c r="T6" s="2">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="U6">
+        <v>5.99</v>
+      </c>
+      <c r="V6" t="s">
+        <v>27</v>
+      </c>
+      <c r="W6">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Scanned. Before Repeater Test
</commit_message>
<xml_diff>
--- a/StockPredictor/bin/Debug/Packages/Data/BIIB/BIIBBag.xlsx
+++ b/StockPredictor/bin/Debug/Packages/Data/BIIB/BIIBBag.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="32">
   <si>
     <t>Date</t>
   </si>
@@ -439,7 +439,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y7"/>
+  <dimension ref="A1:Y8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A3" activeCellId="1" sqref="A2:XFD2 A3:XFD3"/>
@@ -994,6 +994,83 @@
       <c r="W7">
         <v>0</v>
       </c>
+      <c r="X7">
+        <v>-3.5699769999999944</v>
+      </c>
+      <c r="Y7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>42649.8909375</v>
+      </c>
+      <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="C8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8">
+        <v>40</v>
+      </c>
+      <c r="E8">
+        <v>31470</v>
+      </c>
+      <c r="F8">
+        <v>3785</v>
+      </c>
+      <c r="G8">
+        <v>59</v>
+      </c>
+      <c r="H8">
+        <v>39</v>
+      </c>
+      <c r="I8">
+        <v>84</v>
+      </c>
+      <c r="J8">
+        <v>14</v>
+      </c>
+      <c r="K8">
+        <v>29646</v>
+      </c>
+      <c r="L8">
+        <v>457</v>
+      </c>
+      <c r="M8">
+        <v>301</v>
+      </c>
+      <c r="N8">
+        <v>175</v>
+      </c>
+      <c r="O8">
+        <v>30</v>
+      </c>
+      <c r="P8" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q8">
+        <v>49.72799223503381</v>
+      </c>
+      <c r="R8">
+        <v>0</v>
+      </c>
+      <c r="S8" s="2">
+        <v>0.1095</v>
+      </c>
+      <c r="T8" s="2">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="U8">
+        <v>5.95</v>
+      </c>
+      <c r="V8" t="s">
+        <v>27</v>
+      </c>
+      <c r="W8">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
tested repeat trader. Seems to work here. Might still have some problems on the slower computer
</commit_message>
<xml_diff>
--- a/StockPredictor/bin/Debug/Packages/Data/BIIB/BIIBBag.xlsx
+++ b/StockPredictor/bin/Debug/Packages/Data/BIIB/BIIBBag.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="32">
   <si>
     <t>Date</t>
   </si>
@@ -439,7 +439,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y9"/>
+  <dimension ref="A1:Y10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A3" activeCellId="1" sqref="A2:XFD2 A3:XFD3"/>
@@ -447,19 +447,19 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.25" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.25" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.25">
@@ -1148,6 +1148,83 @@
       <c r="W9">
         <v>0</v>
       </c>
+      <c r="X9">
+        <v>-1.7200020000000222</v>
+      </c>
+      <c r="Y9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>42653.880208333336</v>
+      </c>
+      <c r="B10">
+        <v>3</v>
+      </c>
+      <c r="C10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10">
+        <v>24</v>
+      </c>
+      <c r="E10">
+        <v>14696</v>
+      </c>
+      <c r="F10">
+        <v>1939</v>
+      </c>
+      <c r="G10">
+        <v>66</v>
+      </c>
+      <c r="H10">
+        <v>32</v>
+      </c>
+      <c r="I10">
+        <v>83</v>
+      </c>
+      <c r="J10">
+        <v>15</v>
+      </c>
+      <c r="K10">
+        <v>8869</v>
+      </c>
+      <c r="L10">
+        <v>196</v>
+      </c>
+      <c r="M10">
+        <v>95</v>
+      </c>
+      <c r="N10">
+        <v>68</v>
+      </c>
+      <c r="O10">
+        <v>13</v>
+      </c>
+      <c r="P10" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q10">
+        <v>44.409433632991338</v>
+      </c>
+      <c r="R10">
+        <v>1.8</v>
+      </c>
+      <c r="S10" s="2">
+        <v>9.2600000000000002E-2</v>
+      </c>
+      <c r="T10" s="2">
+        <v>-9.4000000000000004E-3</v>
+      </c>
+      <c r="U10">
+        <v>5.87</v>
+      </c>
+      <c r="V10" t="s">
+        <v>27</v>
+      </c>
+      <c r="W10">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
traded, fixed issues with the repeater
</commit_message>
<xml_diff>
--- a/StockPredictor/bin/Debug/Packages/Data/BIIB/BIIBBag.xlsx
+++ b/StockPredictor/bin/Debug/Packages/Data/BIIB/BIIBBag.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="32">
   <si>
     <t>Date</t>
   </si>
@@ -439,7 +439,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y10"/>
+  <dimension ref="A1:Y11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A3" activeCellId="1" sqref="A2:XFD2 A3:XFD3"/>
@@ -1225,6 +1225,83 @@
       <c r="W10">
         <v>0</v>
       </c>
+      <c r="X10">
+        <v>-3.4100040000000149</v>
+      </c>
+      <c r="Y10" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>42654.886678240742</v>
+      </c>
+      <c r="B11">
+        <v>7</v>
+      </c>
+      <c r="C11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11">
+        <v>24</v>
+      </c>
+      <c r="E11">
+        <v>34692</v>
+      </c>
+      <c r="F11">
+        <v>3963</v>
+      </c>
+      <c r="G11">
+        <v>60</v>
+      </c>
+      <c r="H11">
+        <v>37</v>
+      </c>
+      <c r="I11">
+        <v>89</v>
+      </c>
+      <c r="J11">
+        <v>10</v>
+      </c>
+      <c r="K11">
+        <v>27129</v>
+      </c>
+      <c r="L11">
+        <v>338</v>
+      </c>
+      <c r="M11">
+        <v>209</v>
+      </c>
+      <c r="N11">
+        <v>94</v>
+      </c>
+      <c r="O11">
+        <v>11</v>
+      </c>
+      <c r="P11" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q11">
+        <v>39.313912976930268</v>
+      </c>
+      <c r="R11">
+        <v>1.8</v>
+      </c>
+      <c r="S11" s="2">
+        <v>8.6400000000000005E-2</v>
+      </c>
+      <c r="T11" s="2">
+        <v>-1.15E-2</v>
+      </c>
+      <c r="U11">
+        <v>5.85</v>
+      </c>
+      <c r="V11" t="s">
+        <v>27</v>
+      </c>
+      <c r="W11">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>